<commit_message>
Agregue campo Transportista en modulo ReporteVencimientoVo.cs
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteVencimiento.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteVencimiento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\LogicTracker\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias Alfano\Source\Repos\Logictracker 4.0\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,21 +15,22 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$7:$F$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$7:$G$7</definedName>
     <definedName name="CODE">Informe!$C$7</definedName>
     <definedName name="DESCRIPCION">Informe!$D$7</definedName>
-    <definedName name="DIAS_AL_VENCIMIENTO">Informe!$F$7</definedName>
+    <definedName name="DIAS_AL_VENCIMIENTO">Informe!$G$7</definedName>
     <definedName name="PARENTI03">Informe!$B$7</definedName>
     <definedName name="PARENTI25">Informe!$A$7</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
-    <definedName name="VENCIMIENTO">Informe!$E$7</definedName>
+    <definedName name="TRANSPORTISTA">Informe!$E$7</definedName>
+    <definedName name="VENCIMIENTO">Informe!$F$7</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Funciones</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>Días al Vencimiento</t>
+  </si>
+  <si>
+    <t>Transportista</t>
   </si>
 </sst>
 </file>
@@ -995,10 +999,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,12 +1010,12 @@
     <col min="1" max="1" width="25" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1019,44 +1023,50 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1070,22 +1080,26 @@
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:F7"/>
+  <autoFilter ref="A7:G7"/>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="18" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
CAMBIOS EN RESUMEN DE RUTAS Y VENCIMIENTO DOCUMENTOS
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteVencimiento.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteVencimiento.xlsx
@@ -15,22 +15,23 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$7:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$7:$H$7</definedName>
     <definedName name="CODE">Informe!$C$7</definedName>
     <definedName name="DESCRIPCION">Informe!$D$7</definedName>
-    <definedName name="DIAS_AL_VENCIMIENTO">Informe!$G$7</definedName>
+    <definedName name="DIAS_AL_VENCIMIENTO">Informe!$H$7</definedName>
     <definedName name="PARENTI03">Informe!$B$7</definedName>
     <definedName name="PARENTI25">Informe!$A$7</definedName>
+    <definedName name="PRESENTACION">Informe!$F$7</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
     <definedName name="TRANSPORTISTA">Informe!$E$7</definedName>
-    <definedName name="VENCIMIENTO">Informe!$F$7</definedName>
+    <definedName name="VENCIMIENTO">Informe!$G$7</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Funciones</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>Transportista</t>
+  </si>
+  <si>
+    <t>Presentación</t>
   </si>
 </sst>
 </file>
@@ -999,10 +1003,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,12 +1014,12 @@
     <col min="1" max="1" width="25" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1024,40 +1028,45 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1065,8 +1074,9 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1083,23 +1093,27 @@
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:G7"/>
+  <autoFilter ref="A7:H7"/>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="18" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>